<commit_message>
adapted to a large file with a single salary column
</commit_message>
<xml_diff>
--- a/Report/report.xlsx
+++ b/Report/report.xlsx
@@ -473,16 +473,16 @@
         <v>2007</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38916</v>
+        <v>44214</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>40641</v>
+        <v>50240</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2196</v>
+        <v>35341</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>34</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3">
@@ -490,16 +490,16 @@
         <v>2008</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43646</v>
+        <v>48536</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>48428</v>
+        <v>48737</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17549</v>
+        <v>46657</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>196</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4">
@@ -507,16 +507,16 @@
         <v>2009</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>42492</v>
+        <v>44810</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>48109</v>
+        <v>47379</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17709</v>
+        <v>31081</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>171</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
         <v>2010</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43846</v>
+        <v>44648</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>49577</v>
+        <v>48679</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>29093</v>
+        <v>51686</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>328</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6">
@@ -541,16 +541,16 @@
         <v>2011</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>47451</v>
+        <v>46478</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>52794</v>
+        <v>53581</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>36700</v>
+        <v>77413</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>418</v>
+        <v>840</v>
       </c>
     </row>
     <row r="7">
@@ -558,16 +558,16 @@
         <v>2012</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>48243</v>
+        <v>47924</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>58341</v>
+        <v>61113</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44153</v>
+        <v>95147</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>374</v>
+        <v>945</v>
       </c>
     </row>
     <row r="8">
@@ -575,16 +575,16 @@
         <v>2013</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>51510</v>
+        <v>53506</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>57004</v>
+        <v>58409</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>59954</v>
+        <v>129472</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>420</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="9">
@@ -592,16 +592,16 @@
         <v>2014</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>50658</v>
+        <v>49197</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>58768</v>
+        <v>57885</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>66837</v>
+        <v>141481</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>504</v>
+        <v>1250</v>
       </c>
     </row>
   </sheetData>
@@ -658,111 +658,111 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>Минск</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>65722</v>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Москва</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>57354</v>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>45.81%</t>
+          <t>42.58%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>59186</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
           <t>Санкт-Петербург</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>46291</v>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>14.15%</t>
+          <t>12.51%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>41580</v>
+        <v>47008</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Минск</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>2.69%</t>
+          <t>2.74%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>41091</v>
+        <v>42055</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>2.66%</t>
+          <t>2.57%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>41172</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
           <t>Казань</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>37587</v>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>Ростов-на-Дону</t>
-        </is>
-      </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>2.34%</t>
+          <t>2.35%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>34091</v>
+        <v>40003</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
@@ -771,67 +771,67 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>2.02%</t>
+          <t>1.86%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Алматы</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>33637</v>
+        <v>35147</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>1.43%</t>
+          <t>1.81%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Ярославль</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>32744</v>
+        <v>33339</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Воронеж</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>1.4%</t>
+          <t>1.64%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Краснодар</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>32542</v>
+        <v>33023</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>1.33%</t>
+          <t>1.47%</t>
         </is>
       </c>
     </row>

</xml_diff>